<commit_message>
Second Commit without Extent
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>TestCase</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Passwords</t>
   </si>
   <si>
-    <t>jaga@298</t>
+    <t>jaga@2983</t>
   </si>
 </sst>
 </file>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +430,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Third commit with Createccount page with DP
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateAccount" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>TestCase</t>
   </si>
@@ -31,13 +32,76 @@
     <t>SignIn</t>
   </si>
   <si>
-    <t>testjaga002@gmail.com</t>
-  </si>
-  <si>
-    <t>Passwords</t>
-  </si>
-  <si>
-    <t>jaga@2983</t>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DateofBirth</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>TelPhoneNo</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>CreateAccount</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Company </t>
+  </si>
+  <si>
+    <t>Sholinganallur</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>jaga@12345</t>
+  </si>
+  <si>
+    <t>08/29/1993</t>
+  </si>
+  <si>
+    <t>testjaga006@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -82,9 +146,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -390,16 +455,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -413,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -424,33 +490,144 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <v>600119</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2">
+        <v>1234567890</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
+    <hyperlink ref="O2" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fourth Commit with Pos and Negative scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>TestCase</t>
   </si>
@@ -101,7 +101,10 @@
     <t>08/29/1993</t>
   </si>
   <si>
-    <t>testjaga006@gmail.com</t>
+    <t>testjaga007@gmail.com</t>
+  </si>
+  <si>
+    <t>jaga@1234</t>
   </si>
 </sst>
 </file>
@@ -457,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +496,7 @@
         <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -509,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fifth Commit with Comments
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>TestCase</t>
   </si>
@@ -101,10 +101,22 @@
     <t>08/29/1993</t>
   </si>
   <si>
-    <t>testjaga007@gmail.com</t>
-  </si>
-  <si>
     <t>jaga@1234</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>08/30/1993</t>
+  </si>
+  <si>
+    <t>Mahabalipuram</t>
+  </si>
+  <si>
+    <t>testjaga6717@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -458,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,16 +505,32 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -510,10 +538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +622,7 @@
         <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -615,12 +643,59 @@
         <v>25</v>
       </c>
       <c r="M2">
-        <v>1234567890</v>
+        <v>9878653421</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3">
+        <v>600120</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3">
+        <v>9876543211</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -629,8 +704,11 @@
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="N2" r:id="rId2"/>
     <hyperlink ref="O2" r:id="rId3"/>
+    <hyperlink ref="N3" r:id="rId4"/>
+    <hyperlink ref="O3" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Seventh Commit with Documentation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -29,94 +29,94 @@
     <t>Y</t>
   </si>
   <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DateofBirth</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>TelPhoneNo</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>CreateAccount</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Company </t>
+  </si>
+  <si>
+    <t>Sholinganallur</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>jaga@12345</t>
+  </si>
+  <si>
+    <t>08/29/1993</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>08/30/1993</t>
+  </si>
+  <si>
+    <t>Mahabalipuram</t>
+  </si>
+  <si>
     <t>SignIn</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>DateofBirth</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Zipcode</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>TelPhoneNo</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ConfirmPassword</t>
-  </si>
-  <si>
-    <t>CreateAccount</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Company </t>
-  </si>
-  <si>
-    <t>Sholinganallur</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>jaga@12345</t>
-  </si>
-  <si>
-    <t>08/29/1993</t>
+    <t>testjaga8717@gmail.com</t>
   </si>
   <si>
     <t>jaga@1234</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Son</t>
-  </si>
-  <si>
-    <t>08/30/1993</t>
-  </si>
-  <si>
-    <t>Mahabalipuram</t>
-  </si>
-  <si>
-    <t>testjaga6717@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -502,13 +502,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,19 +516,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="D3" r:id="rId3"/>
     <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,43 +566,43 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
-      </c>
-      <c r="O1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -610,46 +610,46 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
       </c>
       <c r="I2">
         <v>600119</v>
       </c>
       <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
       </c>
       <c r="M2">
         <v>9878653421</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -657,46 +657,46 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
       </c>
       <c r="I3">
         <v>600120</v>
       </c>
       <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
       </c>
       <c r="M3">
         <v>9876543211</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
11th Commit with logs
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -107,16 +107,16 @@
     <t>08/30/1993</t>
   </si>
   <si>
-    <t>Mahabalipuram</t>
-  </si>
-  <si>
     <t>SignIn</t>
   </si>
   <si>
-    <t>testjaga8717@gmail.com</t>
-  </si>
-  <si>
     <t>jaga@1234</t>
+  </si>
+  <si>
+    <t>Siruseri</t>
+  </si>
+  <si>
+    <t>testjaga137171@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -148,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -156,15 +156,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -473,13 +490,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -502,10 +519,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
@@ -516,20 +533,20 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
     <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -540,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,11 +567,12 @@
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,7 +640,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
@@ -630,7 +648,7 @@
       <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>600119</v>
       </c>
       <c r="J2" t="s">
@@ -642,8 +660,8 @@
       <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="M2">
-        <v>9878653421</v>
+      <c r="M2" s="2">
+        <v>9876543211</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>25</v>
@@ -669,16 +687,16 @@
         <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3">
-        <v>600120</v>
+        <v>32</v>
+      </c>
+      <c r="I3" s="4">
+        <v>600119</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
@@ -689,7 +707,7 @@
       <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="2">
         <v>9876543211</v>
       </c>
       <c r="N3" s="1" t="s">

</xml_diff>

<commit_message>
12th Commit with ExcelCorrection
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
@@ -15,20 +15,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
   <si>
     <t>TestCase</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>RunMode</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
+    <t>SignIn</t>
+  </si>
+  <si>
+    <t>jaga@12345</t>
+  </si>
+  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -62,9 +71,6 @@
     <t>TelPhoneNo</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>ConfirmPassword</t>
   </si>
   <si>
@@ -77,46 +83,43 @@
     <t>Smith</t>
   </si>
   <si>
-    <t xml:space="preserve">Software Company </t>
+    <t>IT Company</t>
   </si>
   <si>
     <t>Sholinganallur</t>
   </si>
   <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
+    <t>chennai</t>
+  </si>
+  <si>
+    <t>TamilNadu</t>
   </si>
   <si>
     <t>India</t>
   </si>
   <si>
-    <t>jaga@12345</t>
-  </si>
-  <si>
     <t>08/29/1993</t>
   </si>
   <si>
+    <t>600119</t>
+  </si>
+  <si>
+    <t>9876543211</t>
+  </si>
+  <si>
+    <t>08/30/1993</t>
+  </si>
+  <si>
     <t>Jack</t>
   </si>
   <si>
     <t>Son</t>
   </si>
   <si>
-    <t>08/30/1993</t>
-  </si>
-  <si>
-    <t>SignIn</t>
+    <t>testjaga14717@gmail.com</t>
   </si>
   <si>
     <t>jaga@1234</t>
-  </si>
-  <si>
-    <t>Siruseri</t>
-  </si>
-  <si>
-    <t>testjaga137171@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -140,35 +143,26 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -180,8 +174,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -489,65 +483,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -557,164 +550,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
+      <c r="O1" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="3">
-        <v>600119</v>
+        <v>23</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="2">
-        <v>9876543211</v>
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="4">
-        <v>600119</v>
+        <v>23</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="2">
-        <v>9876543211</v>
+        <v>26</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Single TestScript updated Commit
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>RunMode</t>
   </si>
@@ -74,52 +74,40 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
+    <t>IT Company</t>
+  </si>
+  <si>
+    <t>Sholinganallur</t>
+  </si>
+  <si>
+    <t>TamilNadu</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>600119</t>
+  </si>
+  <si>
+    <t>Jaga</t>
+  </si>
+  <si>
+    <t>Waran</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>testjaga277171@gmail.com</t>
+  </si>
+  <si>
     <t>CreateAccount</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>IT Company</t>
-  </si>
-  <si>
-    <t>Sholinganallur</t>
-  </si>
-  <si>
-    <t>chennai</t>
-  </si>
-  <si>
-    <t>TamilNadu</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>08/29/1993</t>
-  </si>
-  <si>
-    <t>600119</t>
-  </si>
-  <si>
-    <t>9876543211</t>
-  </si>
-  <si>
-    <t>08/30/1993</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Son</t>
-  </si>
-  <si>
-    <t>jaga@1234</t>
-  </si>
-  <si>
-    <t>testjaga157176@gmail.com</t>
+    <t>9876543212</t>
+  </si>
+  <si>
+    <t>08/30/1991</t>
   </si>
 </sst>
 </file>
@@ -174,8 +162,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,16 +482,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -515,32 +503,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -548,10 +520,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,49 +544,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -623,105 +595,55 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="O2" r:id="rId2"/>
-    <hyperlink ref="N3" r:id="rId3"/>
-    <hyperlink ref="O3" r:id="rId4"/>
-    <hyperlink ref="F2" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
+    <hyperlink ref="O2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>